<commit_message>
revise and resubmit Democratization
Changes R&R Democratization
</commit_message>
<xml_diff>
--- a/Output/Tables/Model 1a.xlsx
+++ b/Output/Tables/Model 1a.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -411,18 +411,18 @@
         </is>
       </c>
       <c r="B2">
-        <v>1.909</v>
+        <v>2.007</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.135538439536458</t>
+          <t>0.109786837851994</t>
         </is>
       </c>
       <c r="D2">
-        <v>0.142301092922968</v>
+        <v>0.1250748451902961</v>
       </c>
       <c r="E2">
-        <v>18058</v>
+        <v>17877</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -430,10 +430,10 @@
         </is>
       </c>
       <c r="G2">
-        <v>1.674914702141718</v>
+        <v>1.801251879661963</v>
       </c>
       <c r="H2">
-        <v>2.143085297858282</v>
+        <v>2.212748120338037</v>
       </c>
       <c r="I2">
         <v>6</v>
@@ -446,18 +446,18 @@
         </is>
       </c>
       <c r="B3">
-        <v>-0.651</v>
+        <v>-0.589</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.135538439536458</t>
+          <t>0.109786837851994</t>
         </is>
       </c>
       <c r="D3">
-        <v>0.02928303042742726</v>
+        <v>0.02900097998158037</v>
       </c>
       <c r="E3">
-        <v>18058</v>
+        <v>17877</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -465,12 +465,292 @@
         </is>
       </c>
       <c r="G3">
-        <v>-0.6991705850531179</v>
+        <v>-0.6367066120696997</v>
       </c>
       <c r="H3">
-        <v>-0.6028294149468821</v>
+        <v>-0.5412933879303002</v>
       </c>
       <c r="I3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>age</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>-0.007</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0.109786837851994</t>
+        </is>
+      </c>
+      <c r="D4">
+        <v>0.03508013478102524</v>
+      </c>
+      <c r="E4">
+        <v>17877</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Model 1a</t>
+        </is>
+      </c>
+      <c r="G4">
+        <v>-0.06470682171478652</v>
+      </c>
+      <c r="H4">
+        <v>0.05070682171478651</v>
+      </c>
+      <c r="I4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>educ</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>0.173</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0.109786837851994</t>
+        </is>
+      </c>
+      <c r="D5">
+        <v>0.01913072501512775</v>
+      </c>
+      <c r="E5">
+        <v>17877</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Model 1a</t>
+        </is>
+      </c>
+      <c r="G5">
+        <v>0.1415299573501148</v>
+      </c>
+      <c r="H5">
+        <v>0.2044700426498851</v>
+      </c>
+      <c r="I5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>polint</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>-0.355</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0.109786837851994</t>
+        </is>
+      </c>
+      <c r="D6">
+        <v>0.02179640376058222</v>
+      </c>
+      <c r="E6">
+        <v>17877</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Model 1a</t>
+        </is>
+      </c>
+      <c r="G6">
+        <v>-0.3908550841861577</v>
+      </c>
+      <c r="H6">
+        <v>-0.3191449158138422</v>
+      </c>
+      <c r="I6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>sexMale</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>-0.044</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0.109786837851994</t>
+        </is>
+      </c>
+      <c r="D7">
+        <v>0.01297828236770344</v>
+      </c>
+      <c r="E7">
+        <v>17877</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Model 1a</t>
+        </is>
+      </c>
+      <c r="G7">
+        <v>-0.06534927449487216</v>
+      </c>
+      <c r="H7">
+        <v>-0.02265072550512784</v>
+      </c>
+      <c r="I7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>surveyevs2008</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>-0.059</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0.109786837851994</t>
+        </is>
+      </c>
+      <c r="D8">
+        <v>0.01527798735919149</v>
+      </c>
+      <c r="E8">
+        <v>17877</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Model 1a</t>
+        </is>
+      </c>
+      <c r="G8">
+        <v>-0.08413228920587</v>
+      </c>
+      <c r="H8">
+        <v>-0.03386771079412999</v>
+      </c>
+      <c r="I8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>surveywvs1994</t>
+        </is>
+      </c>
+      <c r="B9">
+        <v>-0.15</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>0.109786837851994</t>
+        </is>
+      </c>
+      <c r="D9">
+        <v>0.02556068738474944</v>
+      </c>
+      <c r="E9">
+        <v>17877</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Model 1a</t>
+        </is>
+      </c>
+      <c r="G9">
+        <v>-0.1920473307479128</v>
+      </c>
+      <c r="H9">
+        <v>-0.1079526692520872</v>
+      </c>
+      <c r="I9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>surveywvs1999</t>
+        </is>
+      </c>
+      <c r="B10">
+        <v>0.068</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0.109786837851994</t>
+        </is>
+      </c>
+      <c r="D10">
+        <v>0.03369779570038187</v>
+      </c>
+      <c r="E10">
+        <v>17877</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Model 1a</t>
+        </is>
+      </c>
+      <c r="G10">
+        <v>0.01256712607287182</v>
+      </c>
+      <c r="H10">
+        <v>0.1234328739271282</v>
+      </c>
+      <c r="I10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>surveywvs2005</t>
+        </is>
+      </c>
+      <c r="B11">
+        <v>0.399</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>0.109786837851994</t>
+        </is>
+      </c>
+      <c r="D11">
+        <v>0.02192011013000984</v>
+      </c>
+      <c r="E11">
+        <v>17877</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Model 1a</t>
+        </is>
+      </c>
+      <c r="G11">
+        <v>0.3629414188361338</v>
+      </c>
+      <c r="H11">
+        <v>0.4350585811638662</v>
+      </c>
+      <c r="I11">
         <v>6</v>
       </c>
     </row>

</xml_diff>